<commit_message>
updates initial experiment params
</commit_message>
<xml_diff>
--- a/results/angles_nihavent.xlsx
+++ b/results/angles_nihavent.xlsx
@@ -540,58 +540,58 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>117.4</v>
+        <v>127.5</v>
       </c>
       <c r="D2" t="n">
-        <v>74.09999999999999</v>
+        <v>98</v>
       </c>
       <c r="E2" t="n">
-        <v>107.7</v>
+        <v>119.8</v>
       </c>
       <c r="F2" t="n">
-        <v>52.9</v>
+        <v>56.5</v>
       </c>
       <c r="G2" t="n">
-        <v>43.5</v>
+        <v>37.2</v>
       </c>
       <c r="H2" t="n">
-        <v>79.90000000000001</v>
+        <v>65.8</v>
       </c>
       <c r="I2" t="n">
-        <v>110.9</v>
+        <v>121.4</v>
       </c>
       <c r="J2" t="n">
-        <v>76</v>
+        <v>85.8</v>
       </c>
       <c r="K2" t="n">
-        <v>77.90000000000001</v>
+        <v>90.5</v>
       </c>
       <c r="L2" t="n">
-        <v>94.90000000000001</v>
+        <v>86.90000000000001</v>
       </c>
       <c r="M2" t="n">
-        <v>99.59999999999999</v>
+        <v>105.3</v>
       </c>
       <c r="N2" t="n">
-        <v>118.9</v>
+        <v>119.8</v>
       </c>
       <c r="O2" t="n">
-        <v>108.9</v>
+        <v>102.8</v>
       </c>
       <c r="P2" t="n">
-        <v>90</v>
+        <v>82.3</v>
       </c>
       <c r="Q2" t="n">
-        <v>100</v>
+        <v>96.3</v>
       </c>
       <c r="R2" t="n">
-        <v>92</v>
+        <v>100.2</v>
       </c>
       <c r="S2" t="n">
-        <v>128.4</v>
+        <v>122</v>
       </c>
       <c r="T2" t="n">
-        <v>108.5</v>
+        <v>124.7</v>
       </c>
     </row>
     <row r="3">
@@ -601,61 +601,61 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>117.4</v>
+        <v>127.5</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>84.7</v>
+        <v>76.7</v>
       </c>
       <c r="E3" t="n">
-        <v>42.2</v>
+        <v>43.1</v>
       </c>
       <c r="F3" t="n">
-        <v>117.6</v>
+        <v>118.6</v>
       </c>
       <c r="G3" t="n">
-        <v>102</v>
+        <v>113.5</v>
       </c>
       <c r="H3" t="n">
-        <v>99.40000000000001</v>
+        <v>107.2</v>
       </c>
       <c r="I3" t="n">
-        <v>45.9</v>
+        <v>44.6</v>
       </c>
       <c r="J3" t="n">
-        <v>112.8</v>
+        <v>102.6</v>
       </c>
       <c r="K3" t="n">
-        <v>114.6</v>
+        <v>110.1</v>
       </c>
       <c r="L3" t="n">
-        <v>81.09999999999999</v>
+        <v>85.09999999999999</v>
       </c>
       <c r="M3" t="n">
-        <v>115.3</v>
+        <v>110.3</v>
       </c>
       <c r="N3" t="n">
-        <v>106.7</v>
+        <v>100.9</v>
       </c>
       <c r="O3" t="n">
-        <v>79.3</v>
+        <v>77.7</v>
       </c>
       <c r="P3" t="n">
-        <v>108.3</v>
+        <v>111.9</v>
       </c>
       <c r="Q3" t="n">
-        <v>99.2</v>
+        <v>96.3</v>
       </c>
       <c r="R3" t="n">
-        <v>130.9</v>
+        <v>111.2</v>
       </c>
       <c r="S3" t="n">
-        <v>70.40000000000001</v>
+        <v>52.7</v>
       </c>
       <c r="T3" t="n">
-        <v>107.5</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4">
@@ -665,61 +665,61 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>74.09999999999999</v>
+        <v>98</v>
       </c>
       <c r="C4" t="n">
-        <v>84.7</v>
+        <v>76.7</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>50</v>
+        <v>35.9</v>
       </c>
       <c r="F4" t="n">
-        <v>39.4</v>
+        <v>51.6</v>
       </c>
       <c r="G4" t="n">
-        <v>103.1</v>
+        <v>122.1</v>
       </c>
       <c r="H4" t="n">
-        <v>107.2</v>
+        <v>128</v>
       </c>
       <c r="I4" t="n">
-        <v>84.8</v>
+        <v>74.7</v>
       </c>
       <c r="J4" t="n">
-        <v>108.3</v>
+        <v>113.5</v>
       </c>
       <c r="K4" t="n">
-        <v>75.2</v>
+        <v>87.40000000000001</v>
       </c>
       <c r="L4" t="n">
-        <v>119.9</v>
+        <v>118.2</v>
       </c>
       <c r="M4" t="n">
-        <v>107.7</v>
+        <v>110.6</v>
       </c>
       <c r="N4" t="n">
-        <v>101</v>
+        <v>95.40000000000001</v>
       </c>
       <c r="O4" t="n">
-        <v>108.9</v>
+        <v>105.8</v>
       </c>
       <c r="P4" t="n">
-        <v>114.1</v>
+        <v>129.3</v>
       </c>
       <c r="Q4" t="n">
-        <v>112.8</v>
+        <v>102.5</v>
       </c>
       <c r="R4" t="n">
-        <v>100.7</v>
+        <v>94.8</v>
       </c>
       <c r="S4" t="n">
-        <v>114.5</v>
+        <v>114.2</v>
       </c>
       <c r="T4" t="n">
-        <v>89.90000000000001</v>
+        <v>61.9</v>
       </c>
     </row>
     <row r="5">
@@ -729,61 +729,61 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>107.7</v>
+        <v>119.8</v>
       </c>
       <c r="C5" t="n">
-        <v>42.2</v>
+        <v>43.1</v>
       </c>
       <c r="D5" t="n">
-        <v>50</v>
+        <v>35.9</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>83.5</v>
+        <v>83</v>
       </c>
       <c r="G5" t="n">
-        <v>120.8</v>
+        <v>133.8</v>
       </c>
       <c r="H5" t="n">
-        <v>117.5</v>
+        <v>131.2</v>
       </c>
       <c r="I5" t="n">
-        <v>58.1</v>
+        <v>51.7</v>
       </c>
       <c r="J5" t="n">
-        <v>121.4</v>
+        <v>111</v>
       </c>
       <c r="K5" t="n">
-        <v>105.6</v>
+        <v>101.6</v>
       </c>
       <c r="L5" t="n">
-        <v>102.2</v>
+        <v>108.2</v>
       </c>
       <c r="M5" t="n">
-        <v>125.2</v>
+        <v>117.9</v>
       </c>
       <c r="N5" t="n">
-        <v>105.5</v>
+        <v>99.2</v>
       </c>
       <c r="O5" t="n">
-        <v>86.40000000000001</v>
+        <v>93.5</v>
       </c>
       <c r="P5" t="n">
-        <v>133</v>
+        <v>137.1</v>
       </c>
       <c r="Q5" t="n">
-        <v>111.2</v>
+        <v>105.4</v>
       </c>
       <c r="R5" t="n">
-        <v>119.2</v>
+        <v>102.9</v>
       </c>
       <c r="S5" t="n">
-        <v>90.59999999999999</v>
+        <v>87.3</v>
       </c>
       <c r="T5" t="n">
-        <v>97.5</v>
+        <v>66.2</v>
       </c>
     </row>
     <row r="6">
@@ -793,61 +793,61 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>52.9</v>
+        <v>56.5</v>
       </c>
       <c r="C6" t="n">
-        <v>117.6</v>
+        <v>118.6</v>
       </c>
       <c r="D6" t="n">
-        <v>39.4</v>
+        <v>51.6</v>
       </c>
       <c r="E6" t="n">
-        <v>83.5</v>
+        <v>83</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>84.40000000000001</v>
+        <v>83.09999999999999</v>
       </c>
       <c r="H6" t="n">
-        <v>95.09999999999999</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="I6" t="n">
-        <v>114</v>
+        <v>110.4</v>
       </c>
       <c r="J6" t="n">
-        <v>103.1</v>
+        <v>111.4</v>
       </c>
       <c r="K6" t="n">
-        <v>58.2</v>
+        <v>69.8</v>
       </c>
       <c r="L6" t="n">
-        <v>113</v>
+        <v>109.2</v>
       </c>
       <c r="M6" t="n">
-        <v>97.3</v>
+        <v>107.8</v>
       </c>
       <c r="N6" t="n">
-        <v>97.90000000000001</v>
+        <v>102.8</v>
       </c>
       <c r="O6" t="n">
-        <v>115.8</v>
+        <v>125.2</v>
       </c>
       <c r="P6" t="n">
-        <v>95.8</v>
+        <v>99.40000000000001</v>
       </c>
       <c r="Q6" t="n">
-        <v>107.1</v>
+        <v>100.4</v>
       </c>
       <c r="R6" t="n">
-        <v>88.3</v>
+        <v>92.90000000000001</v>
       </c>
       <c r="S6" t="n">
-        <v>125.3</v>
+        <v>132.4</v>
       </c>
       <c r="T6" t="n">
-        <v>94.8</v>
+        <v>92.40000000000001</v>
       </c>
     </row>
     <row r="7">
@@ -857,61 +857,61 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>43.5</v>
+        <v>37.2</v>
       </c>
       <c r="C7" t="n">
-        <v>102</v>
+        <v>113.5</v>
       </c>
       <c r="D7" t="n">
-        <v>103.1</v>
+        <v>122.1</v>
       </c>
       <c r="E7" t="n">
-        <v>120.8</v>
+        <v>133.8</v>
       </c>
       <c r="F7" t="n">
-        <v>84.40000000000001</v>
+        <v>83.09999999999999</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>71.40000000000001</v>
+        <v>49.1</v>
       </c>
       <c r="I7" t="n">
-        <v>101.3</v>
+        <v>116.3</v>
       </c>
       <c r="J7" t="n">
-        <v>73.59999999999999</v>
+        <v>86.2</v>
       </c>
       <c r="K7" t="n">
-        <v>75.8</v>
+        <v>86.3</v>
       </c>
       <c r="L7" t="n">
-        <v>69.8</v>
+        <v>70.40000000000001</v>
       </c>
       <c r="M7" t="n">
-        <v>87.5</v>
+        <v>91.40000000000001</v>
       </c>
       <c r="N7" t="n">
-        <v>105.1</v>
+        <v>110.6</v>
       </c>
       <c r="O7" t="n">
-        <v>89.3</v>
+        <v>92.09999999999999</v>
       </c>
       <c r="P7" t="n">
-        <v>65.59999999999999</v>
+        <v>53.6</v>
       </c>
       <c r="Q7" t="n">
-        <v>87.5</v>
+        <v>85</v>
       </c>
       <c r="R7" t="n">
-        <v>96.40000000000001</v>
+        <v>109.7</v>
       </c>
       <c r="S7" t="n">
-        <v>92.7</v>
+        <v>90.90000000000001</v>
       </c>
       <c r="T7" t="n">
-        <v>108.9</v>
+        <v>142.4</v>
       </c>
     </row>
     <row r="8">
@@ -921,61 +921,61 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>79.90000000000001</v>
+        <v>65.8</v>
       </c>
       <c r="C8" t="n">
-        <v>99.40000000000001</v>
+        <v>107.2</v>
       </c>
       <c r="D8" t="n">
-        <v>107.2</v>
+        <v>128</v>
       </c>
       <c r="E8" t="n">
-        <v>117.5</v>
+        <v>131.2</v>
       </c>
       <c r="F8" t="n">
-        <v>95.09999999999999</v>
+        <v>98.40000000000001</v>
       </c>
       <c r="G8" t="n">
-        <v>71.40000000000001</v>
+        <v>49.1</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>128.5</v>
+        <v>138.8</v>
       </c>
       <c r="J8" t="n">
-        <v>104.9</v>
+        <v>101.7</v>
       </c>
       <c r="K8" t="n">
-        <v>97.90000000000001</v>
+        <v>93.90000000000001</v>
       </c>
       <c r="L8" t="n">
-        <v>64.3</v>
+        <v>53.7</v>
       </c>
       <c r="M8" t="n">
-        <v>69.90000000000001</v>
+        <v>73</v>
       </c>
       <c r="N8" t="n">
-        <v>105.2</v>
+        <v>108.9</v>
       </c>
       <c r="O8" t="n">
-        <v>114.9</v>
+        <v>93.2</v>
       </c>
       <c r="P8" t="n">
-        <v>54.9</v>
+        <v>57.3</v>
       </c>
       <c r="Q8" t="n">
-        <v>47.9</v>
+        <v>51.1</v>
       </c>
       <c r="R8" t="n">
-        <v>86.3</v>
+        <v>81.40000000000001</v>
       </c>
       <c r="S8" t="n">
-        <v>107</v>
+        <v>89.09999999999999</v>
       </c>
       <c r="T8" t="n">
-        <v>111.6</v>
+        <v>122.8</v>
       </c>
     </row>
     <row r="9">
@@ -985,61 +985,61 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>110.9</v>
+        <v>121.4</v>
       </c>
       <c r="C9" t="n">
-        <v>45.9</v>
+        <v>44.6</v>
       </c>
       <c r="D9" t="n">
-        <v>84.8</v>
+        <v>74.7</v>
       </c>
       <c r="E9" t="n">
-        <v>58.1</v>
+        <v>51.7</v>
       </c>
       <c r="F9" t="n">
-        <v>114</v>
+        <v>110.4</v>
       </c>
       <c r="G9" t="n">
-        <v>101.3</v>
+        <v>116.3</v>
       </c>
       <c r="H9" t="n">
-        <v>128.5</v>
+        <v>138.8</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>74.90000000000001</v>
+        <v>70.59999999999999</v>
       </c>
       <c r="K9" t="n">
-        <v>94.5</v>
+        <v>92</v>
       </c>
       <c r="L9" t="n">
-        <v>106.8</v>
+        <v>113.8</v>
       </c>
       <c r="M9" t="n">
-        <v>108.4</v>
+        <v>105.8</v>
       </c>
       <c r="N9" t="n">
-        <v>87.8</v>
+        <v>84.3</v>
       </c>
       <c r="O9" t="n">
-        <v>78.7</v>
+        <v>81.09999999999999</v>
       </c>
       <c r="P9" t="n">
-        <v>107.2</v>
+        <v>111.9</v>
       </c>
       <c r="Q9" t="n">
-        <v>126.4</v>
+        <v>130.8</v>
       </c>
       <c r="R9" t="n">
-        <v>119.2</v>
+        <v>109.3</v>
       </c>
       <c r="S9" t="n">
-        <v>62.8</v>
+        <v>60.8</v>
       </c>
       <c r="T9" t="n">
-        <v>86.7</v>
+        <v>72.59999999999999</v>
       </c>
     </row>
     <row r="10">
@@ -1049,61 +1049,61 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>76</v>
+        <v>85.8</v>
       </c>
       <c r="C10" t="n">
-        <v>112.8</v>
+        <v>102.6</v>
       </c>
       <c r="D10" t="n">
-        <v>108.3</v>
+        <v>113.5</v>
       </c>
       <c r="E10" t="n">
-        <v>121.4</v>
+        <v>111</v>
       </c>
       <c r="F10" t="n">
-        <v>103.1</v>
+        <v>111.4</v>
       </c>
       <c r="G10" t="n">
+        <v>86.2</v>
+      </c>
+      <c r="H10" t="n">
+        <v>101.7</v>
+      </c>
+      <c r="I10" t="n">
+        <v>70.59999999999999</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>87.59999999999999</v>
+      </c>
+      <c r="L10" t="n">
+        <v>108.1</v>
+      </c>
+      <c r="M10" t="n">
+        <v>76.2</v>
+      </c>
+      <c r="N10" t="n">
+        <v>75.7</v>
+      </c>
+      <c r="O10" t="n">
+        <v>77.90000000000001</v>
+      </c>
+      <c r="P10" t="n">
+        <v>89.5</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>118.7</v>
+      </c>
+      <c r="R10" t="n">
         <v>73.59999999999999</v>
       </c>
-      <c r="H10" t="n">
-        <v>104.9</v>
-      </c>
-      <c r="I10" t="n">
-        <v>74.90000000000001</v>
-      </c>
-      <c r="J10" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" t="n">
-        <v>83.3</v>
-      </c>
-      <c r="L10" t="n">
-        <v>104.7</v>
-      </c>
-      <c r="M10" t="n">
-        <v>73.40000000000001</v>
-      </c>
-      <c r="N10" t="n">
-        <v>73</v>
-      </c>
-      <c r="O10" t="n">
-        <v>79.8</v>
-      </c>
-      <c r="P10" t="n">
-        <v>83.8</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>99.09999999999999</v>
-      </c>
-      <c r="R10" t="n">
-        <v>67.7</v>
-      </c>
       <c r="S10" t="n">
-        <v>81.5</v>
+        <v>86.8</v>
       </c>
       <c r="T10" t="n">
-        <v>61.7</v>
+        <v>74.8</v>
       </c>
     </row>
     <row r="11">
@@ -1113,61 +1113,61 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>77.90000000000001</v>
+        <v>90.5</v>
       </c>
       <c r="C11" t="n">
-        <v>114.6</v>
+        <v>110.1</v>
       </c>
       <c r="D11" t="n">
-        <v>75.2</v>
+        <v>87.40000000000001</v>
       </c>
       <c r="E11" t="n">
-        <v>105.6</v>
+        <v>101.6</v>
       </c>
       <c r="F11" t="n">
-        <v>58.2</v>
+        <v>69.8</v>
       </c>
       <c r="G11" t="n">
-        <v>75.8</v>
+        <v>86.3</v>
       </c>
       <c r="H11" t="n">
-        <v>97.90000000000001</v>
+        <v>93.90000000000001</v>
       </c>
       <c r="I11" t="n">
-        <v>94.5</v>
+        <v>92</v>
       </c>
       <c r="J11" t="n">
-        <v>83.3</v>
+        <v>87.59999999999999</v>
       </c>
       <c r="K11" t="n">
         <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>114.4</v>
+        <v>117.4</v>
       </c>
       <c r="M11" t="n">
-        <v>65.59999999999999</v>
+        <v>66.40000000000001</v>
       </c>
       <c r="N11" t="n">
-        <v>67.8</v>
+        <v>76.40000000000001</v>
       </c>
       <c r="O11" t="n">
-        <v>105.2</v>
+        <v>136.8</v>
       </c>
       <c r="P11" t="n">
-        <v>57.5</v>
+        <v>57.8</v>
       </c>
       <c r="Q11" t="n">
-        <v>112.4</v>
+        <v>107.6</v>
       </c>
       <c r="R11" t="n">
-        <v>91.5</v>
+        <v>82.7</v>
       </c>
       <c r="S11" t="n">
-        <v>84.5</v>
+        <v>83.7</v>
       </c>
       <c r="T11" t="n">
-        <v>81</v>
+        <v>83.40000000000001</v>
       </c>
     </row>
     <row r="12">
@@ -1177,61 +1177,61 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>94.90000000000001</v>
+        <v>86.90000000000001</v>
       </c>
       <c r="C12" t="n">
-        <v>81.09999999999999</v>
+        <v>85.09999999999999</v>
       </c>
       <c r="D12" t="n">
-        <v>119.9</v>
+        <v>118.2</v>
       </c>
       <c r="E12" t="n">
-        <v>102.2</v>
+        <v>108.2</v>
       </c>
       <c r="F12" t="n">
-        <v>113</v>
+        <v>109.2</v>
       </c>
       <c r="G12" t="n">
-        <v>69.8</v>
+        <v>70.40000000000001</v>
       </c>
       <c r="H12" t="n">
-        <v>64.3</v>
+        <v>53.7</v>
       </c>
       <c r="I12" t="n">
-        <v>106.8</v>
+        <v>113.8</v>
       </c>
       <c r="J12" t="n">
-        <v>104.7</v>
+        <v>108.1</v>
       </c>
       <c r="K12" t="n">
-        <v>114.4</v>
+        <v>117.4</v>
       </c>
       <c r="L12" t="n">
         <v>0</v>
       </c>
       <c r="M12" t="n">
-        <v>99.8</v>
+        <v>100</v>
       </c>
       <c r="N12" t="n">
-        <v>85.09999999999999</v>
+        <v>84.90000000000001</v>
       </c>
       <c r="O12" t="n">
-        <v>66.90000000000001</v>
+        <v>62.1</v>
       </c>
       <c r="P12" t="n">
-        <v>74.59999999999999</v>
+        <v>74.8</v>
       </c>
       <c r="Q12" t="n">
-        <v>48.5</v>
+        <v>45.3</v>
       </c>
       <c r="R12" t="n">
-        <v>79.59999999999999</v>
+        <v>85.2</v>
       </c>
       <c r="S12" t="n">
-        <v>66.5</v>
+        <v>68.8</v>
       </c>
       <c r="T12" t="n">
-        <v>103.7</v>
+        <v>125.3</v>
       </c>
     </row>
     <row r="13">
@@ -1241,61 +1241,61 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>99.59999999999999</v>
+        <v>105.3</v>
       </c>
       <c r="C13" t="n">
-        <v>115.3</v>
+        <v>110.3</v>
       </c>
       <c r="D13" t="n">
-        <v>107.7</v>
+        <v>110.6</v>
       </c>
       <c r="E13" t="n">
-        <v>125.2</v>
+        <v>117.9</v>
       </c>
       <c r="F13" t="n">
-        <v>97.3</v>
+        <v>107.8</v>
       </c>
       <c r="G13" t="n">
-        <v>87.5</v>
+        <v>91.40000000000001</v>
       </c>
       <c r="H13" t="n">
-        <v>69.90000000000001</v>
+        <v>73</v>
       </c>
       <c r="I13" t="n">
-        <v>108.4</v>
+        <v>105.8</v>
       </c>
       <c r="J13" t="n">
-        <v>73.40000000000001</v>
+        <v>76.2</v>
       </c>
       <c r="K13" t="n">
-        <v>65.59999999999999</v>
+        <v>66.40000000000001</v>
       </c>
       <c r="L13" t="n">
-        <v>99.8</v>
+        <v>100</v>
       </c>
       <c r="M13" t="n">
         <v>0</v>
       </c>
       <c r="N13" t="n">
-        <v>64.7</v>
+        <v>64.40000000000001</v>
       </c>
       <c r="O13" t="n">
-        <v>86.7</v>
+        <v>89.09999999999999</v>
       </c>
       <c r="P13" t="n">
-        <v>54.6</v>
+        <v>54.8</v>
       </c>
       <c r="Q13" t="n">
-        <v>65.3</v>
+        <v>69.09999999999999</v>
       </c>
       <c r="R13" t="n">
-        <v>62.5</v>
+        <v>67.90000000000001</v>
       </c>
       <c r="S13" t="n">
-        <v>82.8</v>
+        <v>90.5</v>
       </c>
       <c r="T13" t="n">
-        <v>55.3</v>
+        <v>64.8</v>
       </c>
     </row>
     <row r="14">
@@ -1305,61 +1305,61 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>118.9</v>
+        <v>119.8</v>
       </c>
       <c r="C14" t="n">
-        <v>106.7</v>
+        <v>100.9</v>
       </c>
       <c r="D14" t="n">
-        <v>101</v>
+        <v>95.40000000000001</v>
       </c>
       <c r="E14" t="n">
-        <v>105.5</v>
+        <v>99.2</v>
       </c>
       <c r="F14" t="n">
-        <v>97.90000000000001</v>
+        <v>102.8</v>
       </c>
       <c r="G14" t="n">
-        <v>105.1</v>
+        <v>110.6</v>
       </c>
       <c r="H14" t="n">
-        <v>105.2</v>
+        <v>108.9</v>
       </c>
       <c r="I14" t="n">
-        <v>87.8</v>
+        <v>84.3</v>
       </c>
       <c r="J14" t="n">
-        <v>73</v>
+        <v>75.7</v>
       </c>
       <c r="K14" t="n">
-        <v>67.8</v>
+        <v>76.40000000000001</v>
       </c>
       <c r="L14" t="n">
-        <v>85.09999999999999</v>
+        <v>84.90000000000001</v>
       </c>
       <c r="M14" t="n">
-        <v>64.7</v>
+        <v>64.40000000000001</v>
       </c>
       <c r="N14" t="n">
         <v>0</v>
       </c>
       <c r="O14" t="n">
-        <v>67.8</v>
+        <v>67.5</v>
       </c>
       <c r="P14" t="n">
-        <v>66.7</v>
+        <v>73.2</v>
       </c>
       <c r="Q14" t="n">
-        <v>78.40000000000001</v>
+        <v>77.90000000000001</v>
       </c>
       <c r="R14" t="n">
-        <v>50.9</v>
+        <v>66.59999999999999</v>
       </c>
       <c r="S14" t="n">
-        <v>44.7</v>
+        <v>76</v>
       </c>
       <c r="T14" t="n">
-        <v>44.1</v>
+        <v>64.8</v>
       </c>
     </row>
     <row r="15">
@@ -1369,61 +1369,61 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>108.9</v>
+        <v>102.8</v>
       </c>
       <c r="C15" t="n">
-        <v>79.3</v>
+        <v>77.7</v>
       </c>
       <c r="D15" t="n">
-        <v>108.9</v>
+        <v>105.8</v>
       </c>
       <c r="E15" t="n">
-        <v>86.40000000000001</v>
+        <v>93.5</v>
       </c>
       <c r="F15" t="n">
-        <v>115.8</v>
+        <v>125.2</v>
       </c>
       <c r="G15" t="n">
-        <v>89.3</v>
+        <v>92.09999999999999</v>
       </c>
       <c r="H15" t="n">
-        <v>114.9</v>
+        <v>93.2</v>
       </c>
       <c r="I15" t="n">
-        <v>78.7</v>
+        <v>81.09999999999999</v>
       </c>
       <c r="J15" t="n">
-        <v>79.8</v>
+        <v>77.90000000000001</v>
       </c>
       <c r="K15" t="n">
-        <v>105.2</v>
+        <v>136.8</v>
       </c>
       <c r="L15" t="n">
-        <v>66.90000000000001</v>
+        <v>62.1</v>
       </c>
       <c r="M15" t="n">
-        <v>86.7</v>
+        <v>89.09999999999999</v>
       </c>
       <c r="N15" t="n">
-        <v>67.8</v>
+        <v>67.5</v>
       </c>
       <c r="O15" t="n">
         <v>0</v>
       </c>
       <c r="P15" t="n">
-        <v>105.6</v>
+        <v>94.2</v>
       </c>
       <c r="Q15" t="n">
-        <v>74.09999999999999</v>
+        <v>68.2</v>
       </c>
       <c r="R15" t="n">
-        <v>68.5</v>
+        <v>96</v>
       </c>
       <c r="S15" t="n">
-        <v>52.2</v>
+        <v>80.5</v>
       </c>
       <c r="T15" t="n">
-        <v>57.6</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16">
@@ -1433,61 +1433,61 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>90</v>
+        <v>82.3</v>
       </c>
       <c r="C16" t="n">
-        <v>108.3</v>
+        <v>111.9</v>
       </c>
       <c r="D16" t="n">
-        <v>114.1</v>
+        <v>129.3</v>
       </c>
       <c r="E16" t="n">
-        <v>133</v>
+        <v>137.1</v>
       </c>
       <c r="F16" t="n">
-        <v>95.8</v>
+        <v>99.40000000000001</v>
       </c>
       <c r="G16" t="n">
-        <v>65.59999999999999</v>
+        <v>53.6</v>
       </c>
       <c r="H16" t="n">
-        <v>54.9</v>
+        <v>57.3</v>
       </c>
       <c r="I16" t="n">
-        <v>107.2</v>
+        <v>111.9</v>
       </c>
       <c r="J16" t="n">
-        <v>83.8</v>
+        <v>89.5</v>
       </c>
       <c r="K16" t="n">
-        <v>57.5</v>
+        <v>57.8</v>
       </c>
       <c r="L16" t="n">
-        <v>74.59999999999999</v>
+        <v>74.8</v>
       </c>
       <c r="M16" t="n">
-        <v>54.6</v>
+        <v>54.8</v>
       </c>
       <c r="N16" t="n">
-        <v>66.7</v>
+        <v>73.2</v>
       </c>
       <c r="O16" t="n">
-        <v>105.6</v>
+        <v>94.2</v>
       </c>
       <c r="P16" t="n">
         <v>0</v>
       </c>
       <c r="Q16" t="n">
-        <v>72.3</v>
+        <v>72.59999999999999</v>
       </c>
       <c r="R16" t="n">
-        <v>82.7</v>
+        <v>94.40000000000001</v>
       </c>
       <c r="S16" t="n">
-        <v>71.8</v>
+        <v>69.2</v>
       </c>
       <c r="T16" t="n">
-        <v>92.7</v>
+        <v>113.7</v>
       </c>
     </row>
     <row r="17">
@@ -1497,61 +1497,61 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>100</v>
+        <v>96.3</v>
       </c>
       <c r="C17" t="n">
-        <v>99.2</v>
+        <v>96.3</v>
       </c>
       <c r="D17" t="n">
-        <v>112.8</v>
+        <v>102.5</v>
       </c>
       <c r="E17" t="n">
-        <v>111.2</v>
+        <v>105.4</v>
       </c>
       <c r="F17" t="n">
-        <v>107.1</v>
+        <v>100.4</v>
       </c>
       <c r="G17" t="n">
-        <v>87.5</v>
+        <v>85</v>
       </c>
       <c r="H17" t="n">
-        <v>47.9</v>
+        <v>51.1</v>
       </c>
       <c r="I17" t="n">
-        <v>126.4</v>
+        <v>130.8</v>
       </c>
       <c r="J17" t="n">
-        <v>99.09999999999999</v>
+        <v>118.7</v>
       </c>
       <c r="K17" t="n">
-        <v>112.4</v>
+        <v>107.6</v>
       </c>
       <c r="L17" t="n">
-        <v>48.5</v>
+        <v>45.3</v>
       </c>
       <c r="M17" t="n">
-        <v>65.3</v>
+        <v>69.09999999999999</v>
       </c>
       <c r="N17" t="n">
-        <v>78.40000000000001</v>
+        <v>77.90000000000001</v>
       </c>
       <c r="O17" t="n">
-        <v>74.09999999999999</v>
+        <v>68.2</v>
       </c>
       <c r="P17" t="n">
-        <v>72.3</v>
+        <v>72.59999999999999</v>
       </c>
       <c r="Q17" t="n">
         <v>0</v>
       </c>
       <c r="R17" t="n">
-        <v>52.9</v>
+        <v>73.3</v>
       </c>
       <c r="S17" t="n">
-        <v>83.7</v>
+        <v>91.7</v>
       </c>
       <c r="T17" t="n">
-        <v>76.59999999999999</v>
+        <v>94.90000000000001</v>
       </c>
     </row>
     <row r="18">
@@ -1561,61 +1561,61 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>92</v>
+        <v>100.2</v>
       </c>
       <c r="C18" t="n">
-        <v>130.9</v>
+        <v>111.2</v>
       </c>
       <c r="D18" t="n">
-        <v>100.7</v>
+        <v>94.8</v>
       </c>
       <c r="E18" t="n">
-        <v>119.2</v>
+        <v>102.9</v>
       </c>
       <c r="F18" t="n">
-        <v>88.3</v>
+        <v>92.90000000000001</v>
       </c>
       <c r="G18" t="n">
-        <v>96.40000000000001</v>
+        <v>109.7</v>
       </c>
       <c r="H18" t="n">
-        <v>86.3</v>
+        <v>81.40000000000001</v>
       </c>
       <c r="I18" t="n">
-        <v>119.2</v>
+        <v>109.3</v>
       </c>
       <c r="J18" t="n">
-        <v>67.7</v>
+        <v>73.59999999999999</v>
       </c>
       <c r="K18" t="n">
-        <v>91.5</v>
+        <v>82.7</v>
       </c>
       <c r="L18" t="n">
-        <v>79.59999999999999</v>
+        <v>85.2</v>
       </c>
       <c r="M18" t="n">
-        <v>62.5</v>
+        <v>67.90000000000001</v>
       </c>
       <c r="N18" t="n">
-        <v>50.9</v>
+        <v>66.59999999999999</v>
       </c>
       <c r="O18" t="n">
-        <v>68.5</v>
+        <v>96</v>
       </c>
       <c r="P18" t="n">
-        <v>82.7</v>
+        <v>94.40000000000001</v>
       </c>
       <c r="Q18" t="n">
-        <v>52.9</v>
+        <v>73.3</v>
       </c>
       <c r="R18" t="n">
         <v>0</v>
       </c>
       <c r="S18" t="n">
-        <v>82.8</v>
+        <v>99</v>
       </c>
       <c r="T18" t="n">
-        <v>41.8</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19">
@@ -1625,61 +1625,61 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>128.4</v>
+        <v>122</v>
       </c>
       <c r="C19" t="n">
-        <v>70.40000000000001</v>
+        <v>52.7</v>
       </c>
       <c r="D19" t="n">
-        <v>114.5</v>
+        <v>114.2</v>
       </c>
       <c r="E19" t="n">
-        <v>90.59999999999999</v>
+        <v>87.3</v>
       </c>
       <c r="F19" t="n">
-        <v>125.3</v>
+        <v>132.4</v>
       </c>
       <c r="G19" t="n">
-        <v>92.7</v>
+        <v>90.90000000000001</v>
       </c>
       <c r="H19" t="n">
-        <v>107</v>
+        <v>89.09999999999999</v>
       </c>
       <c r="I19" t="n">
-        <v>62.8</v>
+        <v>60.8</v>
       </c>
       <c r="J19" t="n">
-        <v>81.5</v>
+        <v>86.8</v>
       </c>
       <c r="K19" t="n">
-        <v>84.5</v>
+        <v>83.7</v>
       </c>
       <c r="L19" t="n">
-        <v>66.5</v>
+        <v>68.8</v>
       </c>
       <c r="M19" t="n">
-        <v>82.8</v>
+        <v>90.5</v>
       </c>
       <c r="N19" t="n">
-        <v>44.7</v>
+        <v>76</v>
       </c>
       <c r="O19" t="n">
-        <v>52.2</v>
+        <v>80.5</v>
       </c>
       <c r="P19" t="n">
-        <v>71.8</v>
+        <v>69.2</v>
       </c>
       <c r="Q19" t="n">
-        <v>83.7</v>
+        <v>91.7</v>
       </c>
       <c r="R19" t="n">
-        <v>82.8</v>
+        <v>99</v>
       </c>
       <c r="S19" t="n">
         <v>0</v>
       </c>
       <c r="T19" t="n">
-        <v>69.09999999999999</v>
+        <v>104.7</v>
       </c>
     </row>
     <row r="20">
@@ -1689,58 +1689,58 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>108.5</v>
+        <v>124.7</v>
       </c>
       <c r="C20" t="n">
-        <v>107.5</v>
+        <v>87</v>
       </c>
       <c r="D20" t="n">
-        <v>89.90000000000001</v>
+        <v>61.9</v>
       </c>
       <c r="E20" t="n">
-        <v>97.5</v>
+        <v>66.2</v>
       </c>
       <c r="F20" t="n">
-        <v>94.8</v>
+        <v>92.40000000000001</v>
       </c>
       <c r="G20" t="n">
-        <v>108.9</v>
+        <v>142.4</v>
       </c>
       <c r="H20" t="n">
-        <v>111.6</v>
+        <v>122.8</v>
       </c>
       <c r="I20" t="n">
-        <v>86.7</v>
+        <v>72.59999999999999</v>
       </c>
       <c r="J20" t="n">
-        <v>61.7</v>
+        <v>74.8</v>
       </c>
       <c r="K20" t="n">
-        <v>81</v>
+        <v>83.40000000000001</v>
       </c>
       <c r="L20" t="n">
-        <v>103.7</v>
+        <v>125.3</v>
       </c>
       <c r="M20" t="n">
-        <v>55.3</v>
+        <v>64.8</v>
       </c>
       <c r="N20" t="n">
-        <v>44.1</v>
+        <v>64.8</v>
       </c>
       <c r="O20" t="n">
-        <v>57.6</v>
+        <v>89</v>
       </c>
       <c r="P20" t="n">
-        <v>92.7</v>
+        <v>113.7</v>
       </c>
       <c r="Q20" t="n">
-        <v>76.59999999999999</v>
+        <v>94.90000000000001</v>
       </c>
       <c r="R20" t="n">
-        <v>41.8</v>
+        <v>60</v>
       </c>
       <c r="S20" t="n">
-        <v>69.09999999999999</v>
+        <v>104.7</v>
       </c>
       <c r="T20" t="n">
         <v>0</v>

</xml_diff>